<commit_message>
adding section mappings table:
</commit_message>
<xml_diff>
--- a/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model/tables/Harmonised Dataset Model.xlsx
+++ b/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model/tables/Harmonised Dataset Model.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25703"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadassaf/Google Drive/PhD TelecomParisTech - EURECOM - France 2012-2015/My PhD Documents/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model/tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="232">
   <si>
     <t>title</t>
   </si>
@@ -791,12 +796,30 @@
   <si>
     <t>void:Dataset-&gt;dct:format</t>
   </si>
+  <si>
+    <t>https://github.com/indiedotkim/HCLSDatasetDescriptions</t>
+  </si>
+  <si>
+    <t>http://demo.getdkan.com/data.json/</t>
+  </si>
+  <si>
+    <t>https://www.govdata.de/ckan/api/rest/dataset/stala-sn-service-2072056543</t>
+  </si>
+  <si>
+    <t>https://github.com/NuCivic/open_data_federal_extras</t>
+  </si>
+  <si>
+    <t>https://github.com/NuCivic/open_data_schema_map/blob/master/modules/open_data_schema_pod/data/v1.1/dataset.json</t>
+  </si>
+  <si>
+    <t>https://github.com/okfn/ckanext-rdf/blob/master/ckanext/rdf/vocab.py</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1160,57 +1183,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1231,18 +1203,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1271,6 +1231,69 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1667,31 +1690,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="H8" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="10" width="135.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="135.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -1735,17 +1758,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
       <c r="J2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1755,18 +1778,18 @@
       <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="27" t="s">
         <v>171</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="53" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1778,7 +1801,7 @@
       <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="29" t="s">
         <v>140</v>
       </c>
       <c r="F3" s="9"/>
@@ -1793,18 +1816,18 @@
       <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="48" t="s">
+      <c r="M3" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="27" t="s">
         <v>170</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="32"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="53"/>
       <c r="B4" s="9" t="s">
         <v>40</v>
       </c>
@@ -1827,18 +1850,18 @@
       <c r="L4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M4" s="48" t="s">
+      <c r="M4" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="N4" s="48" t="s">
+      <c r="N4" s="27" t="s">
         <v>172</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="32"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="53"/>
       <c r="B5" s="9" t="s">
         <v>41</v>
       </c>
@@ -1860,8 +1883,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="32"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="53"/>
       <c r="B6" s="9" t="s">
         <v>42</v>
       </c>
@@ -1871,18 +1894,18 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="50" t="s">
+      <c r="G6" s="29" t="s">
         <v>174</v>
       </c>
       <c r="H6" s="9"/>
       <c r="J6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="32"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="53"/>
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
@@ -1892,7 +1915,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="29" t="s">
         <v>175</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -1902,8 +1925,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="32"/>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="53"/>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
@@ -1917,8 +1940,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="32"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="53"/>
       <c r="B9" s="9" t="s">
         <v>45</v>
       </c>
@@ -1928,13 +1951,13 @@
       <c r="D9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="29" t="s">
         <v>173</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -1944,8 +1967,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="32"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="53"/>
       <c r="B10" s="9" t="s">
         <v>0</v>
       </c>
@@ -1955,13 +1978,13 @@
       <c r="D10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="29" t="s">
         <v>175</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -1971,15 +1994,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="32"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="53"/>
       <c r="B11" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="29" t="s">
         <v>206</v>
       </c>
       <c r="G11" s="9"/>
@@ -1988,8 +2011,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="32"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="53"/>
       <c r="B12" s="9" t="s">
         <v>68</v>
       </c>
@@ -2003,58 +2026,67 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="32"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="53"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="F13" s="50" t="s">
+      <c r="F13" s="29" t="s">
         <v>217</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="32"/>
+      <c r="J13" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="53"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="50" t="s">
+      <c r="F14" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="29" t="s">
         <v>176</v>
       </c>
       <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="32"/>
+      <c r="J14" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="53"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="50" t="s">
+      <c r="F15" s="29" t="s">
         <v>219</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="19" t="s">
+      <c r="J15" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="37" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -2066,19 +2098,22 @@
       <c r="D16" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="51" t="s">
+      <c r="E16" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="F16" s="51" t="s">
+      <c r="F16" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="G16" s="53"/>
+      <c r="G16" s="32"/>
       <c r="H16" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="20"/>
+      <c r="J16" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="38"/>
       <c r="B17" s="12" t="s">
         <v>54</v>
       </c>
@@ -2090,9 +2125,12 @@
       <c r="H17" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="20"/>
+      <c r="J17" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="38"/>
       <c r="B18" s="12" t="s">
         <v>55</v>
       </c>
@@ -2100,15 +2138,18 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="51" t="s">
+      <c r="G18" s="30" t="s">
         <v>177</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="20"/>
+      <c r="J18" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="38"/>
       <c r="B19" s="12" t="s">
         <v>44</v>
       </c>
@@ -2118,33 +2159,33 @@
       <c r="D19" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="51" t="s">
+      <c r="E19" s="30" t="s">
         <v>155</v>
       </c>
       <c r="F19" s="12"/>
-      <c r="G19" s="51" t="s">
+      <c r="G19" s="30" t="s">
         <v>178</v>
       </c>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="38"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="51" t="s">
+      <c r="E20" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="51" t="s">
+      <c r="F20" s="30" t="s">
         <v>221</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="20"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="38"/>
       <c r="B21" s="14" t="s">
         <v>119</v>
       </c>
@@ -2157,8 +2198,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="21"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="39"/>
       <c r="B22" s="14"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -2169,8 +2210,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="25" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="43" t="s">
         <v>61</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -2180,13 +2221,13 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="52" t="s">
+      <c r="G23" s="31" t="s">
         <v>179</v>
       </c>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="26"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="44"/>
       <c r="B24" s="8" t="s">
         <v>66</v>
       </c>
@@ -2194,11 +2235,11 @@
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="54"/>
+      <c r="G24" s="33"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="26"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="44"/>
       <c r="B25" s="8" t="s">
         <v>77</v>
       </c>
@@ -2206,19 +2247,19 @@
         <v>77</v>
       </c>
       <c r="D25" s="8"/>
-      <c r="E25" s="52" t="s">
+      <c r="E25" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="F25" s="52" t="s">
+      <c r="F25" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="G25" s="52" t="s">
+      <c r="G25" s="31" t="s">
         <v>180</v>
       </c>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="26"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="44"/>
       <c r="B26" s="8" t="s">
         <v>78</v>
       </c>
@@ -2228,19 +2269,19 @@
       <c r="D26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="52" t="s">
+      <c r="E26" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="F26" s="52" t="s">
+      <c r="F26" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="52" t="s">
+      <c r="G26" s="31" t="s">
         <v>181</v>
       </c>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="26"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="44"/>
       <c r="B27" s="8" t="s">
         <v>49</v>
       </c>
@@ -2253,44 +2294,44 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="26"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="44"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="E28" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="F28" s="52" t="s">
+      <c r="F28" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="G28" s="52" t="s">
+      <c r="G28" s="31" t="s">
         <v>182</v>
       </c>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="27"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="54"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="52" t="s">
+      <c r="E29" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="F29" s="52" t="s">
+      <c r="F29" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="G29" s="52" t="s">
+      <c r="G29" s="31" t="s">
         <v>168</v>
       </c>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="45" t="s">
         <v>80</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -2299,42 +2340,42 @@
       <c r="C30" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="E30" s="49" t="s">
+      <c r="E30" s="28" t="s">
         <v>156</v>
       </c>
       <c r="F30" s="15"/>
-      <c r="G30" s="49" t="s">
+      <c r="G30" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="H30" s="49" t="s">
+      <c r="H30" s="28" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="29"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="46"/>
       <c r="B31" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="49" t="s">
+      <c r="E31" s="28" t="s">
         <v>157</v>
       </c>
       <c r="F31" s="15"/>
-      <c r="G31" s="49" t="s">
+      <c r="G31" s="28" t="s">
         <v>184</v>
       </c>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="29"/>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="46"/>
       <c r="B32" s="15" t="s">
         <v>81</v>
       </c>
@@ -2342,31 +2383,31 @@
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
-      <c r="G32" s="49" t="s">
+      <c r="G32" s="28" t="s">
         <v>185</v>
       </c>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="29"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="46"/>
       <c r="B33" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="F33" s="49" t="s">
+      <c r="F33" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="G33" s="49" t="s">
+      <c r="G33" s="28" t="s">
         <v>186</v>
       </c>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="29"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="46"/>
       <c r="B34" s="15" t="s">
         <v>83</v>
       </c>
@@ -2374,19 +2415,19 @@
         <v>83</v>
       </c>
       <c r="D34" s="15"/>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="F34" s="49" t="s">
+      <c r="F34" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="G34" s="49" t="s">
+      <c r="G34" s="28" t="s">
         <v>187</v>
       </c>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="29"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="46"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
@@ -2397,8 +2438,8 @@
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="29"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="46"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15" t="s">
@@ -2409,8 +2450,8 @@
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="29"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="46"/>
       <c r="B37" s="15" t="s">
         <v>1</v>
       </c>
@@ -2418,255 +2459,255 @@
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
-      <c r="G37" s="49" t="s">
+      <c r="G37" s="28" t="s">
         <v>188</v>
       </c>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75">
-      <c r="A38" s="29"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33" t="s">
+    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="46"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33" t="s">
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="H38" s="33"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75">
-      <c r="A39" s="29"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33" t="s">
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="46"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="H39" s="33"/>
-    </row>
-    <row r="40" spans="1:8" ht="15.75">
-      <c r="A40" s="29"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33" t="s">
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="46"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-    </row>
-    <row r="41" spans="1:8" ht="15.75">
-      <c r="A41" s="29"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33" t="s">
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="46"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-    </row>
-    <row r="42" spans="1:8" ht="15.75">
-      <c r="A42" s="29"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33" t="s">
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="46"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-    </row>
-    <row r="43" spans="1:8" ht="15.75">
-      <c r="A43" s="30"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33" t="s">
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="47"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A44" s="40" t="s">
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38" t="s">
+      <c r="C44" s="21"/>
+      <c r="D44" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E44" s="39" t="s">
+      <c r="E44" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="F44" s="39" t="s">
+      <c r="F44" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="G44" s="39" t="s">
+      <c r="G44" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H44" s="38"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="40"/>
-      <c r="B45" s="37" t="s">
+      <c r="H44" s="21"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="48"/>
+      <c r="B45" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="40"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="39" t="s">
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="22" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="40"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="39" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="48"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="40"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="39" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="48"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="22" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="40"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="39" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="48"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A50" s="41" t="s">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="35" t="s">
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="E50" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="F50" s="35" t="s">
+      <c r="F50" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="G50" s="35" t="s">
+      <c r="G50" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="H50" s="34"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="42"/>
-      <c r="B51" s="36" t="s">
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="50"/>
+      <c r="B51" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="34"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="34"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="42"/>
-      <c r="B52" s="36" t="s">
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="17"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="50"/>
+      <c r="B52" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="34"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="34"/>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="43"/>
-      <c r="B53" s="36" t="s">
+      <c r="C52" s="17"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="17"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="51"/>
+      <c r="B53" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C53" s="34"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="34"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="44" t="s">
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="17"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="B54" s="45" t="s">
+      <c r="B54" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="46"/>
-      <c r="D54" s="47" t="s">
+      <c r="C54" s="25"/>
+      <c r="D54" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="47"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47" t="s">
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="H54" s="46"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="16" t="s">
+      <c r="H54" s="25"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="18"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="22" t="s">
+      <c r="B55" s="35"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="36"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="40" t="s">
         <v>37</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -2676,19 +2717,19 @@
       <c r="D56" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="50" t="s">
+      <c r="E56" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="F56" s="50" t="s">
+      <c r="F56" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="G56" s="50" t="s">
+      <c r="G56" s="29" t="s">
         <v>185</v>
       </c>
       <c r="H56" s="9"/>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="23"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="41"/>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
@@ -2696,13 +2737,13 @@
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="50" t="s">
+      <c r="G57" s="29" t="s">
         <v>188</v>
       </c>
       <c r="H57" s="9"/>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="23"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="41"/>
       <c r="B58" s="9" t="s">
         <v>18</v>
       </c>
@@ -2713,8 +2754,8 @@
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="23"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="41"/>
       <c r="B59" s="9" t="s">
         <v>42</v>
       </c>
@@ -2722,13 +2763,13 @@
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="50" t="s">
+      <c r="G59" s="29" t="s">
         <v>192</v>
       </c>
       <c r="H59" s="9"/>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="23"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="41"/>
       <c r="B60" s="9" t="s">
         <v>20</v>
       </c>
@@ -2736,13 +2777,13 @@
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="50" t="s">
+      <c r="G60" s="29" t="s">
         <v>193</v>
       </c>
       <c r="H60" s="9"/>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="23"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="41"/>
       <c r="B61" s="9" t="s">
         <v>85</v>
       </c>
@@ -2753,8 +2794,8 @@
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="23"/>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="41"/>
       <c r="B62" s="9" t="s">
         <v>41</v>
       </c>
@@ -2765,8 +2806,8 @@
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="23"/>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="41"/>
       <c r="B63" s="9" t="s">
         <v>86</v>
       </c>
@@ -2777,8 +2818,8 @@
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
     </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="23"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="41"/>
       <c r="B64" s="9" t="s">
         <v>87</v>
       </c>
@@ -2789,22 +2830,22 @@
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
     </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="24"/>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="42"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E65" s="50"/>
+      <c r="E65" s="29"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="50" t="s">
+      <c r="G65" s="29" t="s">
         <v>194</v>
       </c>
       <c r="H65" s="9"/>
     </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="25" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="43" t="s">
         <v>61</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -2817,8 +2858,8 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="27"/>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="54"/>
       <c r="B67" s="8" t="s">
         <v>66</v>
       </c>
@@ -2829,20 +2870,20 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="16" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="18"/>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="22" t="s">
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="35"/>
+      <c r="H68" s="36"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="40" t="s">
         <v>56</v>
       </c>
       <c r="B69" s="9" t="s">
@@ -2857,8 +2898,8 @@
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
     </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="23"/>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="41"/>
       <c r="B70" s="9" t="s">
         <v>18</v>
       </c>
@@ -2873,8 +2914,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="23"/>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="41"/>
       <c r="B71" s="9" t="s">
         <v>58</v>
       </c>
@@ -2882,17 +2923,17 @@
         <v>58</v>
       </c>
       <c r="D71" s="9"/>
-      <c r="E71" s="50" t="s">
+      <c r="E71" s="29" t="s">
         <v>159</v>
       </c>
       <c r="F71" s="9"/>
-      <c r="G71" s="50" t="s">
+      <c r="G71" s="29" t="s">
         <v>199</v>
       </c>
       <c r="H71" s="9"/>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="23"/>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="41"/>
       <c r="B72" s="9" t="s">
         <v>41</v>
       </c>
@@ -2905,8 +2946,8 @@
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="23"/>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="41"/>
       <c r="B73" s="9" t="s">
         <v>59</v>
       </c>
@@ -2917,8 +2958,8 @@
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
     </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="23"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="41"/>
       <c r="B74" s="9" t="s">
         <v>1</v>
       </c>
@@ -2928,17 +2969,17 @@
       <c r="D74" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E74" s="50" t="s">
+      <c r="E74" s="29" t="s">
         <v>162</v>
       </c>
       <c r="F74" s="9"/>
-      <c r="G74" s="50" t="s">
+      <c r="G74" s="29" t="s">
         <v>195</v>
       </c>
       <c r="H74" s="9"/>
     </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="23"/>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="41"/>
       <c r="B75" s="9" t="s">
         <v>60</v>
       </c>
@@ -2948,19 +2989,19 @@
       <c r="D75" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E75" s="50" t="s">
+      <c r="E75" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="F75" s="50" t="s">
+      <c r="F75" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="G75" s="50" t="s">
+      <c r="G75" s="29" t="s">
         <v>200</v>
       </c>
       <c r="H75" s="9"/>
     </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="23"/>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="41"/>
       <c r="B76" s="10" t="s">
         <v>71</v>
       </c>
@@ -2970,15 +3011,15 @@
       <c r="D76" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E76" s="50" t="s">
+      <c r="E76" s="29" t="s">
         <v>160</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="23"/>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="41"/>
       <c r="B77" s="9" t="s">
         <v>69</v>
       </c>
@@ -2989,8 +3030,8 @@
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="23"/>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="41"/>
       <c r="B78" s="9" t="s">
         <v>20</v>
       </c>
@@ -3000,19 +3041,19 @@
       <c r="D78" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E78" s="50" t="s">
+      <c r="E78" s="29" t="s">
         <v>161</v>
       </c>
       <c r="F78" s="9"/>
-      <c r="G78" s="50" t="s">
+      <c r="G78" s="29" t="s">
         <v>196</v>
       </c>
       <c r="H78" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="23"/>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="41"/>
       <c r="B79" s="9" t="s">
         <v>74</v>
       </c>
@@ -3023,8 +3064,8 @@
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="23"/>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="41"/>
       <c r="B80" s="9" t="s">
         <v>75</v>
       </c>
@@ -3032,13 +3073,13 @@
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
-      <c r="G80" s="50" t="s">
+      <c r="G80" s="29" t="s">
         <v>197</v>
       </c>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="23"/>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="41"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9" t="s">
@@ -3049,8 +3090,8 @@
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="23"/>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="41"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9" t="s">
@@ -3061,8 +3102,8 @@
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="24"/>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="42"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9" t="s">
@@ -3073,8 +3114,8 @@
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
     </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="19" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="37" t="s">
         <v>52</v>
       </c>
       <c r="B84" s="12" t="s">
@@ -3087,8 +3128,8 @@
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
     </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="20"/>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="38"/>
       <c r="B85" s="12" t="s">
         <v>70</v>
       </c>
@@ -3099,8 +3140,8 @@
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
     </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="20"/>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="38"/>
       <c r="B86" s="12" t="s">
         <v>44</v>
       </c>
@@ -3110,37 +3151,37 @@
       <c r="D86" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E86" s="51" t="s">
+      <c r="E86" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="F86" s="51" t="s">
+      <c r="F86" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="G86" s="51" t="s">
+      <c r="G86" s="30" t="s">
         <v>198</v>
       </c>
       <c r="H86" s="12"/>
     </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="20"/>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="38"/>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E87" s="51" t="s">
+      <c r="E87" s="30" t="s">
         <v>164</v>
       </c>
       <c r="F87" s="12"/>
-      <c r="G87" s="51" t="s">
+      <c r="G87" s="30" t="s">
         <v>201</v>
       </c>
       <c r="H87" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="21"/>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="39"/>
       <c r="B88" s="12" t="s">
         <v>73</v>
       </c>
@@ -3151,8 +3192,8 @@
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
     </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="25" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="43" t="s">
         <v>61</v>
       </c>
       <c r="B89" s="8" t="s">
@@ -3162,11 +3203,11 @@
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
-      <c r="G89" s="54"/>
+      <c r="G89" s="33"/>
       <c r="H89" s="8"/>
     </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="26"/>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="44"/>
       <c r="B90" s="8" t="s">
         <v>49</v>
       </c>
@@ -3179,8 +3220,8 @@
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="26"/>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="44"/>
       <c r="B91" s="8" t="s">
         <v>63</v>
       </c>
@@ -3191,8 +3232,8 @@
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
     </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="26"/>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="44"/>
       <c r="B92" s="8" t="s">
         <v>64</v>
       </c>
@@ -3201,16 +3242,16 @@
       </c>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
-      <c r="F92" s="52"/>
-      <c r="G92" s="52" t="s">
+      <c r="F92" s="31"/>
+      <c r="G92" s="31" t="s">
         <v>203</v>
       </c>
       <c r="H92" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="26"/>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="44"/>
       <c r="B93" s="8" t="s">
         <v>65</v>
       </c>
@@ -3220,15 +3261,15 @@
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
       <c r="F93" s="8"/>
-      <c r="G93" s="52" t="s">
+      <c r="G93" s="31" t="s">
         <v>202</v>
       </c>
       <c r="H93" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
-      <c r="A94" s="26"/>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="44"/>
       <c r="B94" s="8" t="s">
         <v>66</v>
       </c>
@@ -3241,20 +3282,20 @@
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
     </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="16" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="18"/>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="19" t="s">
+      <c r="B95" s="35"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="35"/>
+      <c r="E95" s="35"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="35"/>
+      <c r="H95" s="36"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="37" t="s">
         <v>50</v>
       </c>
       <c r="B96" s="12" t="s">
@@ -3269,8 +3310,8 @@
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
     </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="20"/>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="38"/>
       <c r="B97" s="12" t="s">
         <v>1</v>
       </c>
@@ -3283,8 +3324,8 @@
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
     </row>
-    <row r="98" spans="1:8">
-      <c r="A98" s="20"/>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="38"/>
       <c r="B98" s="12" t="s">
         <v>0</v>
       </c>
@@ -3297,8 +3338,8 @@
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
     </row>
-    <row r="99" spans="1:8">
-      <c r="A99" s="20"/>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="38"/>
       <c r="B99" s="12" t="s">
         <v>47</v>
       </c>
@@ -3311,8 +3352,8 @@
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
     </row>
-    <row r="100" spans="1:8">
-      <c r="A100" s="20"/>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="38"/>
       <c r="B100" s="12" t="s">
         <v>18</v>
       </c>
@@ -3325,8 +3366,8 @@
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
     </row>
-    <row r="101" spans="1:8">
-      <c r="A101" s="20"/>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="38"/>
       <c r="B101" s="12" t="s">
         <v>20</v>
       </c>
@@ -3339,8 +3380,8 @@
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
     </row>
-    <row r="102" spans="1:8">
-      <c r="A102" s="21"/>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="39"/>
       <c r="B102" s="14" t="s">
         <v>122</v>
       </c>
@@ -3351,20 +3392,20 @@
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
     </row>
-    <row r="103" spans="1:8">
-      <c r="A103" s="16" t="s">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B103" s="17"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="17"/>
-      <c r="F103" s="17"/>
-      <c r="G103" s="17"/>
-      <c r="H103" s="18"/>
-    </row>
-    <row r="104" spans="1:8">
-      <c r="A104" s="19" t="s">
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="35"/>
+      <c r="F103" s="35"/>
+      <c r="G103" s="35"/>
+      <c r="H103" s="36"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="37" t="s">
         <v>50</v>
       </c>
       <c r="B104" s="12" t="s">
@@ -3374,29 +3415,29 @@
         <v>48</v>
       </c>
       <c r="D104" s="12"/>
-      <c r="E104" s="51" t="s">
+      <c r="E104" s="30" t="s">
         <v>165</v>
       </c>
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
     </row>
-    <row r="105" spans="1:8">
-      <c r="A105" s="20"/>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="38"/>
       <c r="B105" s="12" t="s">
         <v>46</v>
       </c>
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
-      <c r="E105" s="51" t="s">
+      <c r="E105" s="30" t="s">
         <v>167</v>
       </c>
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
     </row>
-    <row r="106" spans="1:8">
-      <c r="A106" s="20"/>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="38"/>
       <c r="B106" s="12" t="s">
         <v>20</v>
       </c>
@@ -3404,15 +3445,15 @@
         <v>20</v>
       </c>
       <c r="D106" s="12"/>
-      <c r="E106" s="51" t="s">
+      <c r="E106" s="30" t="s">
         <v>166</v>
       </c>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
     </row>
-    <row r="107" spans="1:8">
-      <c r="A107" s="20"/>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="38"/>
       <c r="B107" s="12" t="s">
         <v>41</v>
       </c>
@@ -3423,8 +3464,8 @@
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
     </row>
-    <row r="108" spans="1:8">
-      <c r="A108" s="21"/>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="39"/>
       <c r="B108" s="12" t="s">
         <v>18</v>
       </c>
@@ -3437,7 +3478,7 @@
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
adding hdl.json and editign section4
</commit_message>
<xml_diff>
--- a/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model/tables/Harmonised Dataset Model.xlsx
+++ b/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model/tables/Harmonised Dataset Model.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25703"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadassaf/Google Drive/PhD TelecomParisTech - EURECOM - France 2012-2015/My PhD Documents/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model/tables/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="235">
   <si>
     <t>title</t>
   </si>
@@ -566,9 +561,6 @@
     <t>dcat:Dataset-&gt;dcat:contactPoint-&gt;vcard:fn</t>
   </si>
   <si>
-    <t>dcat:Dataset-&gt;dcat:contactPoint-&gt;vcard:hasEmail</t>
-  </si>
-  <si>
     <t>dcat:Distribution-&gt;dct:format</t>
   </si>
   <si>
@@ -814,14 +806,33 @@
   <si>
     <t>https://github.com/okfn/ckanext-rdf/blob/master/ckanext/rdf/vocab.py</t>
   </si>
+  <si>
+    <t>dcat:Dataset-&gt;dct:publisher</t>
+  </si>
+  <si>
+    <t>void:Dataset-&gt;dct:publisher</t>
+  </si>
+  <si>
+    <t>void:Dataset-&gt;dct:keyword</t>
+  </si>
+  <si>
+    <t>dcat:Dataset-&gt;dcat:contactPoint-&gt;vcard:email</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1090,209 +1101,219 @@
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1688,33 +1709,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O109"/>
+  <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H8" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="10" width="135.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="135.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11" style="1"/>
+    <col min="16" max="16" width="24.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -1757,18 +1779,21 @@
       <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="52" t="s">
+      <c r="P1" s="57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75">
+      <c r="A2" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
       <c r="J2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1778,18 +1803,21 @@
       <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="56" t="s">
         <v>143</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="P2" s="56" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="45" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1820,14 +1848,17 @@
         <v>144</v>
       </c>
       <c r="N3" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
+      <c r="P3" s="56" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="45"/>
       <c r="B4" s="9" t="s">
         <v>40</v>
       </c>
@@ -1854,14 +1885,14 @@
         <v>145</v>
       </c>
       <c r="N4" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="53"/>
+    <row r="5" spans="1:16">
+      <c r="A5" s="45"/>
       <c r="B5" s="9" t="s">
         <v>41</v>
       </c>
@@ -1882,9 +1913,15 @@
       <c r="L5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="53"/>
+      <c r="M5" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="P5" s="56" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="45"/>
       <c r="B6" s="9" t="s">
         <v>42</v>
       </c>
@@ -1895,7 +1932,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H6" s="9"/>
       <c r="J6" s="2" t="s">
@@ -1904,8 +1941,8 @@
       <c r="K6" s="27"/>
       <c r="L6" s="27"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
+    <row r="7" spans="1:16">
+      <c r="A7" s="45"/>
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
@@ -1916,7 +1953,7 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>20</v>
@@ -1925,8 +1962,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
+    <row r="8" spans="1:16">
+      <c r="A8" s="45"/>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
@@ -1940,8 +1977,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
+    <row r="9" spans="1:16">
+      <c r="A9" s="45"/>
       <c r="B9" s="9" t="s">
         <v>45</v>
       </c>
@@ -1955,10 +1992,10 @@
         <v>142</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>1</v>
@@ -1967,8 +2004,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
+    <row r="10" spans="1:16">
+      <c r="A10" s="45"/>
       <c r="B10" s="9" t="s">
         <v>0</v>
       </c>
@@ -1982,10 +2019,10 @@
         <v>141</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>20</v>
@@ -1994,8 +2031,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
+    <row r="11" spans="1:16">
+      <c r="A11" s="45"/>
       <c r="B11" s="9" t="s">
         <v>67</v>
       </c>
@@ -2003,7 +2040,7 @@
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -2011,8 +2048,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
+    <row r="12" spans="1:16">
+      <c r="A12" s="45"/>
       <c r="B12" s="9" t="s">
         <v>68</v>
       </c>
@@ -2026,8 +2063,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
+    <row r="13" spans="1:16">
+      <c r="A13" s="45"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="11" t="s">
@@ -2037,16 +2074,16 @@
         <v>148</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="J13" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="53"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="45"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="11" t="s">
@@ -2056,18 +2093,18 @@
         <v>146</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H14" s="9"/>
       <c r="J14" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="53"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="45"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="11" t="s">
@@ -2077,16 +2114,16 @@
         <v>147</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="J15" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="46" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -2102,18 +2139,18 @@
         <v>151</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="12" t="s">
         <v>124</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="47"/>
       <c r="B17" s="12" t="s">
         <v>54</v>
       </c>
@@ -2126,11 +2163,11 @@
         <v>19</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="47"/>
       <c r="B18" s="12" t="s">
         <v>55</v>
       </c>
@@ -2139,17 +2176,17 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>125</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="38"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="47"/>
       <c r="B19" s="12" t="s">
         <v>44</v>
       </c>
@@ -2164,12 +2201,12 @@
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
+    <row r="20" spans="1:10">
+      <c r="A20" s="47"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
@@ -2179,13 +2216,13 @@
         <v>152</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
+    <row r="21" spans="1:10">
+      <c r="A21" s="47"/>
       <c r="B21" s="14" t="s">
         <v>119</v>
       </c>
@@ -2198,8 +2235,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
+    <row r="22" spans="1:10">
+      <c r="A22" s="48"/>
       <c r="B22" s="14"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -2210,8 +2247,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="43" t="s">
+    <row r="23" spans="1:10">
+      <c r="A23" s="49" t="s">
         <v>61</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -2222,12 +2259,12 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
+    <row r="24" spans="1:10">
+      <c r="A24" s="50"/>
       <c r="B24" s="8" t="s">
         <v>66</v>
       </c>
@@ -2238,8 +2275,8 @@
       <c r="G24" s="33"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
+    <row r="25" spans="1:10">
+      <c r="A25" s="50"/>
       <c r="B25" s="8" t="s">
         <v>77</v>
       </c>
@@ -2248,18 +2285,18 @@
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
+    <row r="26" spans="1:10">
+      <c r="A26" s="50"/>
       <c r="B26" s="8" t="s">
         <v>78</v>
       </c>
@@ -2273,15 +2310,15 @@
         <v>153</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
+    <row r="27" spans="1:10">
+      <c r="A27" s="50"/>
       <c r="B27" s="8" t="s">
         <v>49</v>
       </c>
@@ -2294,8 +2331,8 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
+    <row r="28" spans="1:10">
+      <c r="A28" s="50"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8" t="s">
@@ -2305,15 +2342,15 @@
         <v>154</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G28" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="54"/>
+    <row r="29" spans="1:10">
+      <c r="A29" s="51"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
@@ -2323,15 +2360,15 @@
         <v>150</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G29" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="45" t="s">
+    <row r="30" spans="1:10">
+      <c r="A30" s="37" t="s">
         <v>80</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -2348,14 +2385,14 @@
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H30" s="28" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="46"/>
+    <row r="31" spans="1:10">
+      <c r="A31" s="38"/>
       <c r="B31" s="15" t="s">
         <v>35</v>
       </c>
@@ -2365,17 +2402,17 @@
       <c r="D31" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="28" t="s">
-        <v>157</v>
+      <c r="E31" s="55" t="s">
+        <v>234</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="46"/>
+    <row r="32" spans="1:10">
+      <c r="A32" s="38"/>
       <c r="B32" s="15" t="s">
         <v>81</v>
       </c>
@@ -2384,30 +2421,30 @@
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="46"/>
+    <row r="33" spans="1:8">
+      <c r="A33" s="38"/>
       <c r="B33" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
-      <c r="E33" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="F33" s="28" t="s">
-        <v>211</v>
+      <c r="E33" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="F33" s="55" t="s">
+        <v>210</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="46"/>
+    <row r="34" spans="1:8">
+      <c r="A34" s="38"/>
       <c r="B34" s="15" t="s">
         <v>83</v>
       </c>
@@ -2416,18 +2453,18 @@
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="46"/>
+    <row r="35" spans="1:8">
+      <c r="A35" s="38"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
@@ -2438,8 +2475,8 @@
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="46"/>
+    <row r="36" spans="1:8">
+      <c r="A36" s="38"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15" t="s">
@@ -2450,8 +2487,8 @@
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="46"/>
+    <row r="37" spans="1:8">
+      <c r="A37" s="38"/>
       <c r="B37" s="15" t="s">
         <v>1</v>
       </c>
@@ -2460,12 +2497,12 @@
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
       <c r="G37" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="46"/>
+    <row r="38" spans="1:8" ht="15.75">
+      <c r="A38" s="38"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16" t="s">
@@ -2474,24 +2511,24 @@
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H38" s="16"/>
     </row>
-    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="46"/>
+    <row r="39" spans="1:8" ht="15.75">
+      <c r="A39" s="38"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="46"/>
+    <row r="40" spans="1:8" ht="15.75">
+      <c r="A40" s="38"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
       <c r="D40" s="16" t="s">
@@ -2502,8 +2539,8 @@
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="46"/>
+    <row r="41" spans="1:8" ht="15.75">
+      <c r="A41" s="38"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16" t="s">
@@ -2514,8 +2551,8 @@
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
     </row>
-    <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="46"/>
+    <row r="42" spans="1:8" ht="15.75">
+      <c r="A42" s="38"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16" t="s">
@@ -2526,8 +2563,8 @@
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="47"/>
+    <row r="43" spans="1:8" ht="15.75">
+      <c r="A43" s="39"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16" t="s">
@@ -2538,8 +2575,8 @@
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="48" t="s">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A44" s="40" t="s">
         <v>131</v>
       </c>
       <c r="B44" s="20" t="s">
@@ -2553,15 +2590,15 @@
         <v>149</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H44" s="21"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="48"/>
+    <row r="45" spans="1:8">
+      <c r="A45" s="40"/>
       <c r="B45" s="20" t="s">
         <v>121</v>
       </c>
@@ -2572,8 +2609,8 @@
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="48"/>
+    <row r="46" spans="1:8">
+      <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
@@ -2584,8 +2621,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="48"/>
+    <row r="47" spans="1:8">
+      <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
@@ -2596,8 +2633,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="48"/>
+    <row r="48" spans="1:8">
+      <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
@@ -2608,8 +2645,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="48"/>
+    <row r="49" spans="1:8">
+      <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
@@ -2620,8 +2657,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="49" t="s">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A50" s="41" t="s">
         <v>130</v>
       </c>
       <c r="B50" s="17"/>
@@ -2633,15 +2670,15 @@
         <v>150</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="50"/>
+    <row r="51" spans="1:8">
+      <c r="A51" s="42"/>
       <c r="B51" s="19" t="s">
         <v>117</v>
       </c>
@@ -2652,8 +2689,8 @@
       <c r="G51" s="18"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="50"/>
+    <row r="52" spans="1:8">
+      <c r="A52" s="42"/>
       <c r="B52" s="19" t="s">
         <v>116</v>
       </c>
@@ -2664,8 +2701,8 @@
       <c r="G52" s="18"/>
       <c r="H52" s="17"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="51"/>
+    <row r="53" spans="1:8">
+      <c r="A53" s="43"/>
       <c r="B53" s="19" t="s">
         <v>118</v>
       </c>
@@ -2676,7 +2713,7 @@
       <c r="G53" s="18"/>
       <c r="H53" s="17"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" s="23" t="s">
         <v>136</v>
       </c>
@@ -2690,11 +2727,11 @@
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
       <c r="G54" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H54" s="25"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" s="34" t="s">
         <v>84</v>
       </c>
@@ -2706,8 +2743,8 @@
       <c r="G55" s="35"/>
       <c r="H55" s="36"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="40" t="s">
+    <row r="56" spans="1:8">
+      <c r="A56" s="52" t="s">
         <v>37</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -2718,18 +2755,18 @@
         <v>20</v>
       </c>
       <c r="E56" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="F56" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="F56" s="29" t="s">
-        <v>216</v>
-      </c>
       <c r="G56" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H56" s="9"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="41"/>
+    <row r="57" spans="1:8">
+      <c r="A57" s="53"/>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
@@ -2738,12 +2775,12 @@
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
       <c r="G57" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H57" s="9"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="41"/>
+    <row r="58" spans="1:8">
+      <c r="A58" s="53"/>
       <c r="B58" s="9" t="s">
         <v>18</v>
       </c>
@@ -2754,8 +2791,8 @@
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="41"/>
+    <row r="59" spans="1:8">
+      <c r="A59" s="53"/>
       <c r="B59" s="9" t="s">
         <v>42</v>
       </c>
@@ -2764,12 +2801,12 @@
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H59" s="9"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="41"/>
+    <row r="60" spans="1:8">
+      <c r="A60" s="53"/>
       <c r="B60" s="9" t="s">
         <v>20</v>
       </c>
@@ -2778,12 +2815,12 @@
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
       <c r="G60" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H60" s="9"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="41"/>
+    <row r="61" spans="1:8">
+      <c r="A61" s="53"/>
       <c r="B61" s="9" t="s">
         <v>85</v>
       </c>
@@ -2794,8 +2831,8 @@
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="41"/>
+    <row r="62" spans="1:8">
+      <c r="A62" s="53"/>
       <c r="B62" s="9" t="s">
         <v>41</v>
       </c>
@@ -2806,8 +2843,8 @@
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="41"/>
+    <row r="63" spans="1:8">
+      <c r="A63" s="53"/>
       <c r="B63" s="9" t="s">
         <v>86</v>
       </c>
@@ -2818,8 +2855,8 @@
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="41"/>
+    <row r="64" spans="1:8">
+      <c r="A64" s="53"/>
       <c r="B64" s="9" t="s">
         <v>87</v>
       </c>
@@ -2830,8 +2867,8 @@
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="42"/>
+    <row r="65" spans="1:8">
+      <c r="A65" s="54"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9" t="s">
@@ -2840,12 +2877,12 @@
       <c r="E65" s="29"/>
       <c r="F65" s="9"/>
       <c r="G65" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H65" s="9"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="43" t="s">
+    <row r="66" spans="1:8">
+      <c r="A66" s="49" t="s">
         <v>61</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -2858,8 +2895,8 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="54"/>
+    <row r="67" spans="1:8">
+      <c r="A67" s="51"/>
       <c r="B67" s="8" t="s">
         <v>66</v>
       </c>
@@ -2870,7 +2907,7 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68" s="34" t="s">
         <v>9</v>
       </c>
@@ -2882,8 +2919,8 @@
       <c r="G68" s="35"/>
       <c r="H68" s="36"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="40" t="s">
+    <row r="69" spans="1:8">
+      <c r="A69" s="52" t="s">
         <v>56</v>
       </c>
       <c r="B69" s="9" t="s">
@@ -2898,8 +2935,8 @@
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="41"/>
+    <row r="70" spans="1:8">
+      <c r="A70" s="53"/>
       <c r="B70" s="9" t="s">
         <v>18</v>
       </c>
@@ -2914,8 +2951,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="41"/>
+    <row r="71" spans="1:8">
+      <c r="A71" s="53"/>
       <c r="B71" s="9" t="s">
         <v>58</v>
       </c>
@@ -2924,16 +2961,16 @@
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H71" s="9"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="41"/>
+    <row r="72" spans="1:8">
+      <c r="A72" s="53"/>
       <c r="B72" s="9" t="s">
         <v>41</v>
       </c>
@@ -2946,8 +2983,8 @@
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="41"/>
+    <row r="73" spans="1:8">
+      <c r="A73" s="53"/>
       <c r="B73" s="9" t="s">
         <v>59</v>
       </c>
@@ -2958,8 +2995,8 @@
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="41"/>
+    <row r="74" spans="1:8">
+      <c r="A74" s="53"/>
       <c r="B74" s="9" t="s">
         <v>1</v>
       </c>
@@ -2970,16 +3007,16 @@
         <v>1</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H74" s="9"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="41"/>
+    <row r="75" spans="1:8">
+      <c r="A75" s="53"/>
       <c r="B75" s="9" t="s">
         <v>60</v>
       </c>
@@ -2990,18 +3027,18 @@
         <v>60</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F75" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G75" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H75" s="9"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="41"/>
+    <row r="76" spans="1:8">
+      <c r="A76" s="53"/>
       <c r="B76" s="10" t="s">
         <v>71</v>
       </c>
@@ -3012,14 +3049,14 @@
         <v>113</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="41"/>
+    <row r="77" spans="1:8">
+      <c r="A77" s="53"/>
       <c r="B77" s="9" t="s">
         <v>69</v>
       </c>
@@ -3030,8 +3067,8 @@
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="41"/>
+    <row r="78" spans="1:8">
+      <c r="A78" s="53"/>
       <c r="B78" s="9" t="s">
         <v>20</v>
       </c>
@@ -3042,18 +3079,18 @@
         <v>0</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F78" s="9"/>
       <c r="G78" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H78" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="41"/>
+    <row r="79" spans="1:8">
+      <c r="A79" s="53"/>
       <c r="B79" s="9" t="s">
         <v>74</v>
       </c>
@@ -3064,8 +3101,8 @@
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="41"/>
+    <row r="80" spans="1:8">
+      <c r="A80" s="53"/>
       <c r="B80" s="9" t="s">
         <v>75</v>
       </c>
@@ -3074,12 +3111,12 @@
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
       <c r="G80" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="41"/>
+    <row r="81" spans="1:8">
+      <c r="A81" s="53"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9" t="s">
@@ -3090,8 +3127,8 @@
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="41"/>
+    <row r="82" spans="1:8">
+      <c r="A82" s="53"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9" t="s">
@@ -3102,8 +3139,8 @@
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="42"/>
+    <row r="83" spans="1:8">
+      <c r="A83" s="54"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9" t="s">
@@ -3114,8 +3151,8 @@
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="37" t="s">
+    <row r="84" spans="1:8">
+      <c r="A84" s="46" t="s">
         <v>52</v>
       </c>
       <c r="B84" s="12" t="s">
@@ -3128,8 +3165,8 @@
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="38"/>
+    <row r="85" spans="1:8">
+      <c r="A85" s="47"/>
       <c r="B85" s="12" t="s">
         <v>70</v>
       </c>
@@ -3140,8 +3177,8 @@
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="38"/>
+    <row r="86" spans="1:8">
+      <c r="A86" s="47"/>
       <c r="B86" s="12" t="s">
         <v>44</v>
       </c>
@@ -3152,36 +3189,36 @@
         <v>111</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="F86" s="30" t="s">
-        <v>208</v>
+        <v>162</v>
+      </c>
+      <c r="F86" s="58" t="s">
+        <v>207</v>
       </c>
       <c r="G86" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H86" s="12"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="38"/>
+    <row r="87" spans="1:8">
+      <c r="A87" s="47"/>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12" t="s">
         <v>112</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F87" s="12"/>
       <c r="G87" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H87" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="39"/>
+    <row r="88" spans="1:8">
+      <c r="A88" s="48"/>
       <c r="B88" s="12" t="s">
         <v>73</v>
       </c>
@@ -3192,8 +3229,8 @@
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="43" t="s">
+    <row r="89" spans="1:8">
+      <c r="A89" s="49" t="s">
         <v>61</v>
       </c>
       <c r="B89" s="8" t="s">
@@ -3206,8 +3243,8 @@
       <c r="G89" s="33"/>
       <c r="H89" s="8"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="44"/>
+    <row r="90" spans="1:8">
+      <c r="A90" s="50"/>
       <c r="B90" s="8" t="s">
         <v>49</v>
       </c>
@@ -3220,8 +3257,8 @@
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="44"/>
+    <row r="91" spans="1:8">
+      <c r="A91" s="50"/>
       <c r="B91" s="8" t="s">
         <v>63</v>
       </c>
@@ -3232,8 +3269,8 @@
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="44"/>
+    <row r="92" spans="1:8">
+      <c r="A92" s="50"/>
       <c r="B92" s="8" t="s">
         <v>64</v>
       </c>
@@ -3244,14 +3281,14 @@
       <c r="E92" s="8"/>
       <c r="F92" s="31"/>
       <c r="G92" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H92" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="44"/>
+    <row r="93" spans="1:8">
+      <c r="A93" s="50"/>
       <c r="B93" s="8" t="s">
         <v>65</v>
       </c>
@@ -3262,14 +3299,14 @@
       <c r="E93" s="8"/>
       <c r="F93" s="8"/>
       <c r="G93" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H93" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="44"/>
+    <row r="94" spans="1:8">
+      <c r="A94" s="50"/>
       <c r="B94" s="8" t="s">
         <v>66</v>
       </c>
@@ -3282,7 +3319,7 @@
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8">
       <c r="A95" s="34" t="s">
         <v>38</v>
       </c>
@@ -3294,8 +3331,8 @@
       <c r="G95" s="35"/>
       <c r="H95" s="36"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="37" t="s">
+    <row r="96" spans="1:8">
+      <c r="A96" s="46" t="s">
         <v>50</v>
       </c>
       <c r="B96" s="12" t="s">
@@ -3310,8 +3347,8 @@
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="38"/>
+    <row r="97" spans="1:8">
+      <c r="A97" s="47"/>
       <c r="B97" s="12" t="s">
         <v>1</v>
       </c>
@@ -3324,8 +3361,8 @@
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="38"/>
+    <row r="98" spans="1:8">
+      <c r="A98" s="47"/>
       <c r="B98" s="12" t="s">
         <v>0</v>
       </c>
@@ -3338,8 +3375,8 @@
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="38"/>
+    <row r="99" spans="1:8">
+      <c r="A99" s="47"/>
       <c r="B99" s="12" t="s">
         <v>47</v>
       </c>
@@ -3352,8 +3389,8 @@
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="38"/>
+    <row r="100" spans="1:8">
+      <c r="A100" s="47"/>
       <c r="B100" s="12" t="s">
         <v>18</v>
       </c>
@@ -3366,8 +3403,8 @@
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="38"/>
+    <row r="101" spans="1:8">
+      <c r="A101" s="47"/>
       <c r="B101" s="12" t="s">
         <v>20</v>
       </c>
@@ -3380,8 +3417,8 @@
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="39"/>
+    <row r="102" spans="1:8">
+      <c r="A102" s="48"/>
       <c r="B102" s="14" t="s">
         <v>122</v>
       </c>
@@ -3392,7 +3429,7 @@
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8">
       <c r="A103" s="34" t="s">
         <v>2</v>
       </c>
@@ -3404,8 +3441,8 @@
       <c r="G103" s="35"/>
       <c r="H103" s="36"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="37" t="s">
+    <row r="104" spans="1:8">
+      <c r="A104" s="46" t="s">
         <v>50</v>
       </c>
       <c r="B104" s="12" t="s">
@@ -3416,28 +3453,28 @@
       </c>
       <c r="D104" s="12"/>
       <c r="E104" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="38"/>
+    <row r="105" spans="1:8">
+      <c r="A105" s="47"/>
       <c r="B105" s="12" t="s">
         <v>46</v>
       </c>
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
       <c r="E105" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="38"/>
+    <row r="106" spans="1:8">
+      <c r="A106" s="47"/>
       <c r="B106" s="12" t="s">
         <v>20</v>
       </c>
@@ -3446,14 +3483,14 @@
       </c>
       <c r="D106" s="12"/>
       <c r="E106" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="38"/>
+    <row r="107" spans="1:8">
+      <c r="A107" s="47"/>
       <c r="B107" s="12" t="s">
         <v>41</v>
       </c>
@@ -3464,8 +3501,8 @@
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="39"/>
+    <row r="108" spans="1:8">
+      <c r="A108" s="48"/>
       <c r="B108" s="12" t="s">
         <v>18</v>
       </c>
@@ -3478,7 +3515,7 @@
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8">
       <c r="A109" s="7" t="s">
         <v>51</v>
       </c>
@@ -3494,6 +3531,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A103:H103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A69:A83"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="A89:A94"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A96:A102"/>
     <mergeCell ref="A68:H68"/>
     <mergeCell ref="A30:A43"/>
     <mergeCell ref="A44:A49"/>
@@ -3505,13 +3549,6 @@
     <mergeCell ref="A55:H55"/>
     <mergeCell ref="A56:A65"/>
     <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A103:H103"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="A69:A83"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="A89:A94"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A96:A102"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>